<commit_message>
ADC Module completed. Status updated
</commit_message>
<xml_diff>
--- a/Documentation Status.xlsx
+++ b/Documentation Status.xlsx
@@ -475,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -498,7 +498,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -506,7 +506,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:3">

</xml_diff>

<commit_message>
Solar Panels and Launch adapter files added
</commit_message>
<xml_diff>
--- a/Documentation Status.xlsx
+++ b/Documentation Status.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>Modules</t>
   </si>
@@ -87,9 +87,6 @@
     <t>Data sheets to be added</t>
   </si>
   <si>
-    <t>Needs Radiation Plots etc</t>
-  </si>
-  <si>
     <t>Needs More Info</t>
   </si>
   <si>
@@ -133,6 +130,21 @@
   </si>
   <si>
     <t>Needs pic and note on PTFE insulated wire</t>
+  </si>
+  <si>
+    <t>Solar Panels</t>
+  </si>
+  <si>
+    <t>First Upload of files</t>
+  </si>
+  <si>
+    <t>Launch Adapter</t>
+  </si>
+  <si>
+    <t>Mechanical Drawings uploaded</t>
+  </si>
+  <si>
+    <t>Ant Switch complete, Plots of ants added</t>
   </si>
 </sst>
 </file>
@@ -473,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -498,7 +510,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -506,7 +518,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -514,7 +526,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -522,7 +534,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -538,7 +550,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -546,7 +558,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -562,7 +574,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -570,7 +582,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -578,7 +590,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -586,79 +598,95 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
         <v>20</v>
       </c>
-      <c r="C22" t="s">
-        <v>38</v>
+      <c r="C24" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ADAC Coil Driver, Sun Sensor and GPS files completed
</commit_message>
<xml_diff>
--- a/Documentation Status.xlsx
+++ b/Documentation Status.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t>Modules</t>
   </si>
@@ -90,16 +90,7 @@
     <t>Needs More Info</t>
   </si>
   <si>
-    <t>Delete V1 data</t>
-  </si>
-  <si>
-    <t>Needs Data sheet</t>
-  </si>
-  <si>
     <t>Data doesn't look right</t>
-  </si>
-  <si>
-    <t>Delete Interface RevA</t>
   </si>
   <si>
     <t>Looks to be Rev1 needs to be updated</t>
@@ -488,7 +479,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -510,7 +501,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -518,7 +509,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -526,7 +517,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -550,7 +541,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -558,7 +549,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -566,7 +557,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -574,7 +565,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -598,15 +589,15 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -622,7 +613,7 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -630,7 +621,7 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -638,7 +629,7 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -646,7 +637,7 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -654,23 +645,23 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C21" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C22" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -678,7 +669,7 @@
         <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -686,7 +677,7 @@
         <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reference to dxfViewer added and Status updated
</commit_message>
<xml_diff>
--- a/Documentation Status.xlsx
+++ b/Documentation Status.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>Modules</t>
   </si>
@@ -100,9 +100,6 @@
   </si>
   <si>
     <t>Complete</t>
-  </si>
-  <si>
-    <t>Needs reference to dxf file reader</t>
   </si>
   <si>
     <t xml:space="preserve">Could be deleted or contents moved </t>
@@ -478,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -517,7 +514,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -594,10 +591,10 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
         <v>37</v>
-      </c>
-      <c r="C14" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -629,7 +626,7 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -637,7 +634,7 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -645,23 +642,23 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" t="s">
         <v>31</v>
-      </c>
-      <c r="C21" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" t="s">
         <v>35</v>
-      </c>
-      <c r="C22" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -669,7 +666,7 @@
         <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -677,7 +674,7 @@
         <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pcb Panel Files added to Camera and Magnetometer.
</commit_message>
<xml_diff>
--- a/Documentation Status.xlsx
+++ b/Documentation Status.xlsx
@@ -102,9 +102,6 @@
     <t>Complete</t>
   </si>
   <si>
-    <t xml:space="preserve">Could be deleted or contents moved </t>
-  </si>
-  <si>
     <t>Delete V1 &amp; V2 add more data for V3</t>
   </si>
   <si>
@@ -133,6 +130,9 @@
   </si>
   <si>
     <t>Ant Switch complete, Plots of ants added</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contents moved, folder deleted </t>
   </si>
 </sst>
 </file>
@@ -475,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -514,7 +514,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -591,10 +591,10 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
         <v>36</v>
-      </c>
-      <c r="C14" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -634,7 +634,7 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -642,23 +642,23 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" t="s">
         <v>30</v>
-      </c>
-      <c r="C21" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" t="s">
         <v>34</v>
-      </c>
-      <c r="C22" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -666,7 +666,7 @@
         <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -674,7 +674,7 @@
         <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>